<commit_message>
Quedan registradas todas las estaciones del metro en imagenes, en ubicaciones y en separacion entre estas, y se pasan todos los test propuestos
</commit_message>
<xml_diff>
--- a/procesamiento_datos/datos/procesados/estaciones_separacion.xlsx
+++ b/procesamiento_datos/datos/procesados/estaciones_separacion.xlsx
@@ -1253,7 +1253,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>etiopia/plaza de la transparencia</t>
+          <t>etiopia plaza de la transparencia</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1263,7 +1263,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>etiopia/plaza de la transparencia</t>
+          <t>etiopia plaza de la transparencia</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>viveros/derechos humanos</t>
+          <t>viveros derechos humanos</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1338,7 +1338,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>viveros/derechos humanos</t>
+          <t>viveros derechos humanos</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>etiopia/plaza de la transparencia</t>
+          <t>etiopia plaza de la transparencia</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>etiopia/plaza de la transparencia</t>
+          <t>etiopia plaza de la transparencia</t>
         </is>
       </c>
       <c r="C239" t="n">
@@ -4068,7 +4068,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>viveros/derechos humanos</t>
+          <t>viveros derechos humanos</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>viveros/derechos humanos</t>
+          <t>viveros derechos humanos</t>
         </is>
       </c>
       <c r="C244" t="n">

</xml_diff>